<commit_message>
implemented send email to dc with proper subject and body
implemented send email to dc with proper subject and body
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FamBrands_bot1\Documents\GitHub\Trafficking-Request-Email-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF00C42-6973-4FAE-B96E-13F6B5F0163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B37C25-B2FE-4A7B-9809-F79CA8E5BE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13845" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -168,7 +168,16 @@
     <t>TCDR_EmailReportRecipient</t>
   </si>
   <si>
-    <t>TCDR_ReportMailSubject</t>
+    <t>TCDR_MailReportTransactionSubject</t>
+  </si>
+  <si>
+    <t>TCDR_RequestMailSubject</t>
+  </si>
+  <si>
+    <t>TCDR_CotscoFormOutputPath</t>
+  </si>
+  <si>
+    <t>TCDR_ReportPath</t>
   </si>
 </sst>
 </file>
@@ -2794,13 +2803,12 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="1" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -2854,18 +2862,48 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>